<commit_message>
updates for bot. Building new algorithm
</commit_message>
<xml_diff>
--- a/files/grid.xlsx
+++ b/files/grid.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="SOLUSDT" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -149,7 +149,7 @@
       <selection pane="topLeft" activeCell="D59" activeCellId="0" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.38"/>
   </cols>

</xml_diff>

<commit_message>
removed price updater. Tests was successfully
</commit_message>
<xml_diff>
--- a/files/grid.xlsx
+++ b/files/grid.xlsx
@@ -278,10 +278,10 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.66"/>
@@ -312,7 +312,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="n">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="B2" s="7" t="n">
         <v>72</v>
@@ -329,7 +329,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="n">
-        <v>0.11</v>
+        <v>0.59</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>72</v>
@@ -340,7 +340,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="n">
-        <v>0.12</v>
+        <v>0.58</v>
       </c>
       <c r="B4" s="7" t="n">
         <v>72</v>
@@ -351,7 +351,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="n">
-        <v>0.13</v>
+        <v>0.57</v>
       </c>
       <c r="B5" s="7" t="n">
         <v>72</v>
@@ -362,7 +362,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="n">
-        <v>0.14</v>
+        <v>0.56</v>
       </c>
       <c r="B6" s="7" t="n">
         <v>72</v>
@@ -373,7 +373,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="n">
-        <v>0.15</v>
+        <v>0.55</v>
       </c>
       <c r="B7" s="7" t="n">
         <v>72</v>
@@ -384,7 +384,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="n">
-        <v>0.16</v>
+        <v>0.54</v>
       </c>
       <c r="B8" s="7" t="n">
         <v>72</v>
@@ -395,7 +395,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="n">
-        <v>0.17</v>
+        <v>0.53</v>
       </c>
       <c r="B9" s="7" t="n">
         <v>72</v>
@@ -406,7 +406,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="n">
-        <v>0.18</v>
+        <v>0.52</v>
       </c>
       <c r="B10" s="7" t="n">
         <v>72</v>
@@ -417,7 +417,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="n">
-        <v>0.19</v>
+        <v>0.51</v>
       </c>
       <c r="B11" s="7" t="n">
         <v>72</v>
@@ -428,7 +428,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="B12" s="7" t="n">
         <v>72</v>
@@ -439,7 +439,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
-        <v>0.21</v>
+        <v>0.49</v>
       </c>
       <c r="B13" s="7" t="n">
         <v>72</v>
@@ -450,7 +450,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
-        <v>0.22</v>
+        <v>0.48</v>
       </c>
       <c r="B14" s="7" t="n">
         <v>72</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
-        <v>0.23</v>
+        <v>0.47</v>
       </c>
       <c r="B15" s="7" t="n">
         <v>72</v>
@@ -472,7 +472,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
-        <v>0.24</v>
+        <v>0.46</v>
       </c>
       <c r="B16" s="7" t="n">
         <v>72</v>
@@ -483,49 +483,40 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
-        <v>0.25</v>
+        <v>0.45</v>
       </c>
       <c r="B17" s="7" t="n">
         <v>72</v>
       </c>
       <c r="C17" s="8" t="n">
         <v>70</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="n">
-        <v>0.26</v>
+        <v>0.44</v>
       </c>
       <c r="B18" s="7" t="n">
         <v>72</v>
       </c>
       <c r="C18" s="8" t="n">
         <v>70</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="n">
-        <v>0.27</v>
+        <v>0.43</v>
       </c>
       <c r="B19" s="7" t="n">
         <v>72</v>
       </c>
       <c r="C19" s="8" t="n">
         <v>70</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="n">
-        <v>0.28</v>
+        <v>0.42</v>
       </c>
       <c r="B20" s="7" t="n">
         <v>72</v>
@@ -536,7 +527,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="n">
-        <v>0.29</v>
+        <v>0.41</v>
       </c>
       <c r="B21" s="7" t="n">
         <v>72</v>
@@ -547,7 +538,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="B22" s="7" t="n">
         <v>72</v>
@@ -558,7 +549,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="n">
-        <v>0.31</v>
+        <v>0.39</v>
       </c>
       <c r="B23" s="7" t="n">
         <v>72</v>
@@ -569,7 +560,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="n">
-        <v>0.32</v>
+        <v>0.38</v>
       </c>
       <c r="B24" s="7" t="n">
         <v>72</v>
@@ -580,7 +571,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="n">
-        <v>0.33</v>
+        <v>0.37</v>
       </c>
       <c r="B25" s="7" t="n">
         <v>72</v>
@@ -591,7 +582,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="n">
-        <v>0.34</v>
+        <v>0.36</v>
       </c>
       <c r="B26" s="7" t="n">
         <v>72</v>
@@ -613,7 +604,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="n">
-        <v>0.36</v>
+        <v>0.34</v>
       </c>
       <c r="B28" s="7" t="n">
         <v>72</v>
@@ -624,7 +615,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="n">
-        <v>0.37</v>
+        <v>0.33</v>
       </c>
       <c r="B29" s="7" t="n">
         <v>72</v>
@@ -635,7 +626,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="n">
-        <v>0.38</v>
+        <v>0.32</v>
       </c>
       <c r="B30" s="7" t="n">
         <v>72</v>
@@ -646,7 +637,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="n">
-        <v>0.39</v>
+        <v>0.31</v>
       </c>
       <c r="B31" s="7" t="n">
         <v>72</v>
@@ -657,7 +648,7 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="B32" s="7" t="n">
         <v>72</v>
@@ -668,7 +659,7 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="n">
-        <v>0.41</v>
+        <v>0.29</v>
       </c>
       <c r="B33" s="7" t="n">
         <v>72</v>
@@ -679,7 +670,7 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="n">
-        <v>0.42</v>
+        <v>0.28</v>
       </c>
       <c r="B34" s="7" t="n">
         <v>72</v>
@@ -690,7 +681,7 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="n">
-        <v>0.43</v>
+        <v>0.27</v>
       </c>
       <c r="B35" s="7" t="n">
         <v>72</v>
@@ -701,40 +692,49 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="n">
-        <v>0.44</v>
+        <v>0.26</v>
       </c>
       <c r="B36" s="7" t="n">
         <v>72</v>
       </c>
       <c r="C36" s="8" t="n">
         <v>70</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="n">
-        <v>0.45</v>
+        <v>0.25</v>
       </c>
       <c r="B37" s="7" t="n">
         <v>72</v>
       </c>
       <c r="C37" s="8" t="n">
         <v>70</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="n">
-        <v>0.46</v>
+        <v>0.24</v>
       </c>
       <c r="B38" s="7" t="n">
         <v>72</v>
       </c>
       <c r="C38" s="8" t="n">
         <v>70</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="n">
-        <v>0.47</v>
+        <v>0.23</v>
       </c>
       <c r="B39" s="7" t="n">
         <v>72</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="n">
-        <v>0.48</v>
+        <v>0.22</v>
       </c>
       <c r="B40" s="7" t="n">
         <v>72</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="n">
-        <v>0.49</v>
+        <v>0.21</v>
       </c>
       <c r="B41" s="7" t="n">
         <v>72</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="n">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="B42" s="7" t="n">
         <v>72</v>
@@ -778,7 +778,7 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="n">
-        <v>0.51</v>
+        <v>0.19</v>
       </c>
       <c r="B43" s="7" t="n">
         <v>72</v>
@@ -789,7 +789,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="n">
-        <v>0.52</v>
+        <v>0.18</v>
       </c>
       <c r="B44" s="7" t="n">
         <v>72</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="n">
-        <v>0.53</v>
+        <v>0.17</v>
       </c>
       <c r="B45" s="7" t="n">
         <v>72</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="n">
-        <v>0.54</v>
+        <v>0.16</v>
       </c>
       <c r="B46" s="7" t="n">
         <v>72</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="n">
-        <v>0.55</v>
+        <v>0.15</v>
       </c>
       <c r="B47" s="7" t="n">
         <v>72</v>
@@ -833,7 +833,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="n">
-        <v>0.56</v>
+        <v>0.14</v>
       </c>
       <c r="B48" s="7" t="n">
         <v>72</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="n">
-        <v>0.57</v>
+        <v>0.13</v>
       </c>
       <c r="B49" s="7" t="n">
         <v>72</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="6" t="n">
-        <v>0.58</v>
+        <v>0.12</v>
       </c>
       <c r="B50" s="7" t="n">
         <v>72</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="6" t="n">
-        <v>0.59</v>
+        <v>0.11</v>
       </c>
       <c r="B51" s="7" t="n">
         <v>72</v>

</xml_diff>

<commit_message>
BinanceTrader update orders now saved with orderId
</commit_message>
<xml_diff>
--- a/files/grid.xlsx
+++ b/files/grid.xlsx
@@ -278,10 +278,10 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.66"/>
@@ -324,7 +324,7 @@
         <v>100</v>
       </c>
       <c r="F2" s="4" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
move other buyy into the buy orders
</commit_message>
<xml_diff>
--- a/files/grid.xlsx
+++ b/files/grid.xlsx
@@ -44,7 +44,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -64,6 +64,11 @@
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -116,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -151,19 +156,14 @@
     <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -424,7 +424,7 @@
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="6">
-        <v>95.0</v>
+        <v>90.0</v>
       </c>
       <c r="F2" s="7">
         <v>0.12</v>
@@ -959,9 +959,7 @@
       <c r="C46" s="4">
         <v>3.0</v>
       </c>
-      <c r="D46" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="D46" s="12"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="10">
@@ -973,9 +971,7 @@
       <c r="C47" s="4">
         <v>3.0</v>
       </c>
-      <c r="D47" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D47" s="12"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="10">
@@ -987,9 +983,7 @@
       <c r="C48" s="4">
         <v>3.0</v>
       </c>
-      <c r="D48" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D48" s="12"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
       <c r="A49" s="10">
@@ -1001,9 +995,7 @@
       <c r="C49" s="4">
         <v>3.0</v>
       </c>
-      <c r="D49" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D49" s="12"/>
     </row>
     <row r="50" ht="12.75" customHeight="1">
       <c r="A50" s="10">
@@ -1015,9 +1007,7 @@
       <c r="C50" s="4">
         <v>3.0</v>
       </c>
-      <c r="D50" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D50" s="12"/>
     </row>
     <row r="51" ht="12.75" customHeight="1">
       <c r="A51" s="10">
@@ -1029,9 +1019,7 @@
       <c r="C51" s="4">
         <v>3.0</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D51" s="12"/>
     </row>
     <row r="52" ht="12.75" customHeight="1">
       <c r="A52" s="10">
@@ -1043,9 +1031,7 @@
       <c r="C52" s="4">
         <v>3.0</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D52" s="12"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
       <c r="A53" s="10">
@@ -1057,9 +1043,7 @@
       <c r="C53" s="4">
         <v>3.0</v>
       </c>
-      <c r="D53" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D53" s="12"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
       <c r="A54" s="10">
@@ -1071,9 +1055,7 @@
       <c r="C54" s="4">
         <v>3.0</v>
       </c>
-      <c r="D54" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D54" s="12"/>
     </row>
     <row r="55" ht="12.75" customHeight="1">
       <c r="A55" s="10">
@@ -1085,9 +1067,7 @@
       <c r="C55" s="4">
         <v>3.0</v>
       </c>
-      <c r="D55" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D55" s="12"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
       <c r="A56" s="10">
@@ -1099,9 +1079,7 @@
       <c r="C56" s="4">
         <v>3.0</v>
       </c>
-      <c r="D56" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D56" s="12"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
       <c r="A57" s="10">
@@ -1113,9 +1091,7 @@
       <c r="C57" s="4">
         <v>3.0</v>
       </c>
-      <c r="D57" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D57" s="12"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
       <c r="A58" s="10">
@@ -1223,7 +1199,9 @@
       <c r="C66" s="4">
         <v>3.0</v>
       </c>
-      <c r="D66" s="5"/>
+      <c r="D66" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="67" ht="12.75" customHeight="1">
       <c r="A67" s="10">
@@ -1235,7 +1213,9 @@
       <c r="C67" s="4">
         <v>3.0</v>
       </c>
-      <c r="D67" s="5"/>
+      <c r="D67" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="68" ht="12.75" customHeight="1">
       <c r="A68" s="10">
@@ -1247,7 +1227,9 @@
       <c r="C68" s="4">
         <v>3.0</v>
       </c>
-      <c r="D68" s="5"/>
+      <c r="D68" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="69" ht="12.75" customHeight="1">
       <c r="A69" s="10">
@@ -1259,7 +1241,9 @@
       <c r="C69" s="4">
         <v>3.0</v>
       </c>
-      <c r="D69" s="5"/>
+      <c r="D69" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="70" ht="12.75" customHeight="1">
       <c r="A70" s="10">
@@ -1271,7 +1255,9 @@
       <c r="C70" s="4">
         <v>3.0</v>
       </c>
-      <c r="D70" s="5"/>
+      <c r="D70" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="71" ht="12.75" customHeight="1">
       <c r="A71" s="10">
@@ -1283,7 +1269,9 @@
       <c r="C71" s="4">
         <v>3.0</v>
       </c>
-      <c r="D71" s="5"/>
+      <c r="D71" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="72" ht="12.75" customHeight="1">
       <c r="A72" s="10">
@@ -1295,880 +1283,1132 @@
       <c r="C72" s="4">
         <v>3.0</v>
       </c>
-      <c r="D72" s="5"/>
+      <c r="D72" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="73" ht="12.75" customHeight="1">
-      <c r="A73" s="12"/>
-      <c r="B73" s="4"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="5"/>
+      <c r="A73" s="10">
+        <v>2.39</v>
+      </c>
+      <c r="B73" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C73" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="74" ht="12.75" customHeight="1">
-      <c r="A74" s="12"/>
-      <c r="B74" s="4"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="5"/>
+      <c r="A74" s="10">
+        <v>2.38</v>
+      </c>
+      <c r="B74" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C74" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="75" ht="12.75" customHeight="1">
-      <c r="A75" s="12"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="5"/>
+      <c r="A75" s="10">
+        <v>2.37</v>
+      </c>
+      <c r="B75" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C75" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="76" ht="12.75" customHeight="1">
-      <c r="A76" s="12"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="5"/>
+      <c r="A76" s="10">
+        <v>2.36</v>
+      </c>
+      <c r="B76" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C76" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="77" ht="12.75" customHeight="1">
-      <c r="A77" s="12"/>
-      <c r="B77" s="15"/>
-      <c r="C77" s="16"/>
-      <c r="D77" s="5"/>
+      <c r="A77" s="10">
+        <v>2.35</v>
+      </c>
+      <c r="B77" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C77" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="78" ht="12.75" customHeight="1">
-      <c r="A78" s="12"/>
-      <c r="B78" s="15"/>
-      <c r="C78" s="16"/>
+      <c r="A78" s="10">
+        <v>2.34</v>
+      </c>
+      <c r="B78" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C78" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D78" s="5"/>
     </row>
     <row r="79" ht="12.75" customHeight="1">
-      <c r="A79" s="12"/>
-      <c r="B79" s="15"/>
-      <c r="C79" s="16"/>
+      <c r="A79" s="10">
+        <v>2.33</v>
+      </c>
+      <c r="B79" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C79" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D79" s="5"/>
     </row>
     <row r="80" ht="12.75" customHeight="1">
-      <c r="A80" s="12"/>
-      <c r="B80" s="15"/>
-      <c r="C80" s="16"/>
+      <c r="A80" s="10">
+        <v>2.32</v>
+      </c>
+      <c r="B80" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C80" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D80" s="5"/>
     </row>
     <row r="81" ht="12.75" customHeight="1">
-      <c r="A81" s="12"/>
-      <c r="B81" s="15"/>
-      <c r="C81" s="16"/>
+      <c r="A81" s="10">
+        <v>2.31</v>
+      </c>
+      <c r="B81" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C81" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D81" s="5"/>
     </row>
     <row r="82" ht="12.75" customHeight="1">
-      <c r="A82" s="12"/>
-      <c r="B82" s="15"/>
-      <c r="C82" s="16"/>
+      <c r="A82" s="10">
+        <v>2.3</v>
+      </c>
+      <c r="B82" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C82" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D82" s="5"/>
     </row>
     <row r="83" ht="12.75" customHeight="1">
-      <c r="A83" s="12"/>
-      <c r="B83" s="15"/>
-      <c r="C83" s="16"/>
+      <c r="A83" s="10">
+        <v>2.29</v>
+      </c>
+      <c r="B83" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C83" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D83" s="5"/>
     </row>
     <row r="84" ht="12.75" customHeight="1">
-      <c r="A84" s="12"/>
-      <c r="B84" s="15"/>
-      <c r="C84" s="16"/>
+      <c r="A84" s="10">
+        <v>2.28</v>
+      </c>
+      <c r="B84" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C84" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D84" s="5"/>
     </row>
     <row r="85" ht="12.75" customHeight="1">
-      <c r="A85" s="12"/>
-      <c r="B85" s="15"/>
-      <c r="C85" s="16"/>
+      <c r="A85" s="10">
+        <v>2.27</v>
+      </c>
+      <c r="B85" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C85" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D85" s="5"/>
     </row>
     <row r="86" ht="12.75" customHeight="1">
-      <c r="A86" s="12"/>
-      <c r="B86" s="15"/>
-      <c r="C86" s="16"/>
+      <c r="A86" s="10">
+        <v>2.26</v>
+      </c>
+      <c r="B86" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C86" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D86" s="5"/>
     </row>
     <row r="87" ht="12.75" customHeight="1">
-      <c r="A87" s="12"/>
-      <c r="B87" s="15"/>
-      <c r="C87" s="16"/>
+      <c r="A87" s="10">
+        <v>2.25</v>
+      </c>
+      <c r="B87" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C87" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D87" s="5"/>
     </row>
     <row r="88" ht="12.75" customHeight="1">
-      <c r="A88" s="12"/>
-      <c r="B88" s="15"/>
-      <c r="C88" s="16"/>
+      <c r="A88" s="10">
+        <v>2.24</v>
+      </c>
+      <c r="B88" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C88" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D88" s="5"/>
     </row>
     <row r="89" ht="12.75" customHeight="1">
-      <c r="A89" s="12"/>
-      <c r="B89" s="15"/>
-      <c r="C89" s="16"/>
+      <c r="A89" s="10">
+        <v>2.23</v>
+      </c>
+      <c r="B89" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C89" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D89" s="5"/>
     </row>
     <row r="90" ht="12.75" customHeight="1">
-      <c r="A90" s="12"/>
-      <c r="B90" s="15"/>
-      <c r="C90" s="16"/>
+      <c r="A90" s="10">
+        <v>2.22</v>
+      </c>
+      <c r="B90" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C90" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D90" s="5"/>
     </row>
     <row r="91" ht="12.75" customHeight="1">
-      <c r="A91" s="12"/>
-      <c r="B91" s="15"/>
-      <c r="C91" s="16"/>
+      <c r="A91" s="10">
+        <v>2.21</v>
+      </c>
+      <c r="B91" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C91" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D91" s="5"/>
     </row>
     <row r="92" ht="12.75" customHeight="1">
-      <c r="A92" s="12"/>
-      <c r="B92" s="15"/>
-      <c r="C92" s="16"/>
+      <c r="A92" s="10">
+        <v>2.2</v>
+      </c>
+      <c r="B92" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C92" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D92" s="5"/>
     </row>
     <row r="93" ht="12.75" customHeight="1">
-      <c r="A93" s="12"/>
-      <c r="B93" s="15"/>
-      <c r="C93" s="16"/>
+      <c r="A93" s="10">
+        <v>2.19</v>
+      </c>
+      <c r="B93" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C93" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D93" s="5"/>
     </row>
     <row r="94" ht="12.75" customHeight="1">
-      <c r="A94" s="12"/>
-      <c r="B94" s="15"/>
-      <c r="C94" s="16"/>
+      <c r="A94" s="10">
+        <v>2.18</v>
+      </c>
+      <c r="B94" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C94" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D94" s="5"/>
     </row>
     <row r="95" ht="12.75" customHeight="1">
-      <c r="A95" s="12"/>
-      <c r="B95" s="15"/>
-      <c r="C95" s="16"/>
+      <c r="A95" s="10">
+        <v>2.17</v>
+      </c>
+      <c r="B95" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C95" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D95" s="5"/>
     </row>
     <row r="96" ht="12.75" customHeight="1">
-      <c r="A96" s="12"/>
-      <c r="B96" s="15"/>
-      <c r="C96" s="16"/>
+      <c r="A96" s="10">
+        <v>2.16</v>
+      </c>
+      <c r="B96" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C96" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D96" s="5"/>
     </row>
     <row r="97" ht="12.75" customHeight="1">
-      <c r="A97" s="12"/>
-      <c r="B97" s="15"/>
-      <c r="C97" s="16"/>
+      <c r="A97" s="10">
+        <v>2.15</v>
+      </c>
+      <c r="B97" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C97" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D97" s="5"/>
     </row>
     <row r="98" ht="12.75" customHeight="1">
-      <c r="A98" s="12"/>
-      <c r="B98" s="15"/>
-      <c r="C98" s="16"/>
+      <c r="A98" s="10">
+        <v>2.14</v>
+      </c>
+      <c r="B98" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C98" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D98" s="5"/>
     </row>
     <row r="99" ht="12.75" customHeight="1">
-      <c r="A99" s="12"/>
-      <c r="B99" s="15"/>
-      <c r="C99" s="16"/>
+      <c r="A99" s="10">
+        <v>2.13</v>
+      </c>
+      <c r="B99" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C99" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D99" s="5"/>
     </row>
     <row r="100" ht="12.75" customHeight="1">
-      <c r="A100" s="12"/>
-      <c r="B100" s="15"/>
-      <c r="C100" s="16"/>
+      <c r="A100" s="10">
+        <v>2.12</v>
+      </c>
+      <c r="B100" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C100" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D100" s="5"/>
     </row>
     <row r="101" ht="12.75" customHeight="1">
-      <c r="A101" s="12"/>
-      <c r="B101" s="15"/>
-      <c r="C101" s="16"/>
+      <c r="A101" s="10">
+        <v>2.11</v>
+      </c>
+      <c r="B101" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C101" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D101" s="5"/>
     </row>
     <row r="102" ht="12.75" customHeight="1">
-      <c r="A102" s="12"/>
-      <c r="B102" s="15"/>
-      <c r="C102" s="16"/>
+      <c r="A102" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="B102" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C102" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D102" s="5"/>
     </row>
     <row r="103" ht="12.75" customHeight="1">
-      <c r="A103" s="12"/>
-      <c r="B103" s="15"/>
-      <c r="C103" s="16"/>
+      <c r="A103" s="10">
+        <v>2.09</v>
+      </c>
+      <c r="B103" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C103" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D103" s="5"/>
     </row>
     <row r="104" ht="12.75" customHeight="1">
-      <c r="A104" s="12"/>
-      <c r="B104" s="15"/>
-      <c r="C104" s="16"/>
+      <c r="A104" s="10">
+        <v>2.08</v>
+      </c>
+      <c r="B104" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C104" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D104" s="5"/>
     </row>
     <row r="105" ht="12.75" customHeight="1">
-      <c r="A105" s="12"/>
-      <c r="B105" s="15"/>
-      <c r="C105" s="16"/>
+      <c r="A105" s="10">
+        <v>2.07</v>
+      </c>
+      <c r="B105" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C105" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D105" s="5"/>
     </row>
     <row r="106" ht="12.75" customHeight="1">
-      <c r="A106" s="12"/>
-      <c r="B106" s="15"/>
-      <c r="C106" s="16"/>
+      <c r="A106" s="10">
+        <v>2.06</v>
+      </c>
+      <c r="B106" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C106" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D106" s="5"/>
     </row>
     <row r="107" ht="12.75" customHeight="1">
-      <c r="A107" s="12"/>
-      <c r="B107" s="15"/>
-      <c r="C107" s="16"/>
+      <c r="A107" s="10">
+        <v>2.05</v>
+      </c>
+      <c r="B107" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C107" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D107" s="5"/>
     </row>
     <row r="108" ht="12.75" customHeight="1">
-      <c r="A108" s="12"/>
-      <c r="B108" s="15"/>
-      <c r="C108" s="16"/>
+      <c r="A108" s="10">
+        <v>2.04</v>
+      </c>
+      <c r="B108" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C108" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D108" s="5"/>
     </row>
     <row r="109" ht="12.75" customHeight="1">
-      <c r="A109" s="12"/>
-      <c r="B109" s="15"/>
-      <c r="C109" s="16"/>
+      <c r="A109" s="10">
+        <v>2.03</v>
+      </c>
+      <c r="B109" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C109" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D109" s="5"/>
     </row>
     <row r="110" ht="12.75" customHeight="1">
-      <c r="A110" s="12"/>
-      <c r="B110" s="15"/>
-      <c r="C110" s="16"/>
+      <c r="A110" s="10">
+        <v>2.02</v>
+      </c>
+      <c r="B110" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C110" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D110" s="5"/>
     </row>
     <row r="111" ht="12.75" customHeight="1">
-      <c r="A111" s="12"/>
-      <c r="B111" s="15"/>
-      <c r="C111" s="16"/>
+      <c r="A111" s="10">
+        <v>2.01</v>
+      </c>
+      <c r="B111" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C111" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D111" s="5"/>
     </row>
     <row r="112" ht="12.75" customHeight="1">
-      <c r="A112" s="12"/>
-      <c r="B112" s="15"/>
-      <c r="C112" s="16"/>
+      <c r="A112" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B112" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C112" s="4">
+        <v>3.0</v>
+      </c>
       <c r="D112" s="5"/>
     </row>
     <row r="113" ht="12.75" customHeight="1">
-      <c r="A113" s="12"/>
-      <c r="B113" s="15"/>
-      <c r="C113" s="16"/>
+      <c r="A113" s="13"/>
+      <c r="B113" s="14"/>
+      <c r="C113" s="15"/>
       <c r="D113" s="5"/>
     </row>
     <row r="114" ht="12.75" customHeight="1">
-      <c r="A114" s="12"/>
-      <c r="B114" s="15"/>
-      <c r="C114" s="16"/>
+      <c r="A114" s="13"/>
+      <c r="B114" s="14"/>
+      <c r="C114" s="15"/>
       <c r="D114" s="5"/>
     </row>
     <row r="115" ht="12.75" customHeight="1">
-      <c r="A115" s="12"/>
-      <c r="B115" s="15"/>
-      <c r="C115" s="16"/>
+      <c r="A115" s="13"/>
+      <c r="B115" s="14"/>
+      <c r="C115" s="15"/>
       <c r="D115" s="5"/>
     </row>
     <row r="116" ht="12.75" customHeight="1">
-      <c r="A116" s="12"/>
-      <c r="B116" s="15"/>
-      <c r="C116" s="16"/>
+      <c r="A116" s="13"/>
+      <c r="B116" s="14"/>
+      <c r="C116" s="15"/>
       <c r="D116" s="5"/>
     </row>
     <row r="117" ht="12.75" customHeight="1">
-      <c r="A117" s="12"/>
-      <c r="B117" s="15"/>
-      <c r="C117" s="16"/>
+      <c r="A117" s="13"/>
+      <c r="B117" s="14"/>
+      <c r="C117" s="15"/>
       <c r="D117" s="5"/>
     </row>
     <row r="118" ht="12.75" customHeight="1">
-      <c r="A118" s="12"/>
-      <c r="B118" s="15"/>
-      <c r="C118" s="16"/>
+      <c r="A118" s="13"/>
+      <c r="B118" s="14"/>
+      <c r="C118" s="15"/>
       <c r="D118" s="5"/>
     </row>
     <row r="119" ht="12.75" customHeight="1">
-      <c r="A119" s="12"/>
-      <c r="B119" s="15"/>
-      <c r="C119" s="16"/>
+      <c r="A119" s="13"/>
+      <c r="B119" s="14"/>
+      <c r="C119" s="15"/>
       <c r="D119" s="5"/>
     </row>
     <row r="120" ht="12.75" customHeight="1">
-      <c r="A120" s="12"/>
-      <c r="B120" s="15"/>
-      <c r="C120" s="16"/>
+      <c r="A120" s="13"/>
+      <c r="B120" s="14"/>
+      <c r="C120" s="15"/>
       <c r="D120" s="5"/>
     </row>
     <row r="121" ht="12.75" customHeight="1">
-      <c r="A121" s="12"/>
-      <c r="B121" s="15"/>
-      <c r="C121" s="16"/>
+      <c r="A121" s="13"/>
+      <c r="B121" s="14"/>
+      <c r="C121" s="15"/>
       <c r="D121" s="5"/>
     </row>
     <row r="122" ht="12.75" customHeight="1">
-      <c r="A122" s="12"/>
-      <c r="B122" s="15"/>
-      <c r="C122" s="16"/>
+      <c r="A122" s="13"/>
+      <c r="B122" s="14"/>
+      <c r="C122" s="15"/>
       <c r="D122" s="5"/>
     </row>
     <row r="123" ht="12.75" customHeight="1">
-      <c r="A123" s="12"/>
-      <c r="B123" s="15"/>
-      <c r="C123" s="16"/>
+      <c r="A123" s="13"/>
+      <c r="B123" s="14"/>
+      <c r="C123" s="15"/>
       <c r="D123" s="5"/>
     </row>
     <row r="124" ht="12.75" customHeight="1">
-      <c r="A124" s="12"/>
-      <c r="B124" s="15"/>
-      <c r="C124" s="16"/>
+      <c r="A124" s="13"/>
+      <c r="B124" s="14"/>
+      <c r="C124" s="15"/>
       <c r="D124" s="5"/>
     </row>
     <row r="125" ht="12.75" customHeight="1">
-      <c r="A125" s="12"/>
-      <c r="B125" s="15"/>
-      <c r="C125" s="16"/>
+      <c r="A125" s="13"/>
+      <c r="B125" s="14"/>
+      <c r="C125" s="15"/>
       <c r="D125" s="5"/>
     </row>
     <row r="126" ht="12.75" customHeight="1">
-      <c r="A126" s="12"/>
-      <c r="B126" s="15"/>
-      <c r="C126" s="16"/>
+      <c r="A126" s="13"/>
+      <c r="B126" s="14"/>
+      <c r="C126" s="15"/>
       <c r="D126" s="5"/>
     </row>
     <row r="127" ht="12.75" customHeight="1">
-      <c r="A127" s="12"/>
-      <c r="B127" s="15"/>
-      <c r="C127" s="16"/>
+      <c r="A127" s="13"/>
+      <c r="B127" s="14"/>
+      <c r="C127" s="15"/>
       <c r="D127" s="5"/>
     </row>
     <row r="128" ht="12.75" customHeight="1">
-      <c r="A128" s="12"/>
-      <c r="B128" s="15"/>
-      <c r="C128" s="16"/>
+      <c r="A128" s="13"/>
+      <c r="B128" s="14"/>
+      <c r="C128" s="15"/>
       <c r="D128" s="5"/>
     </row>
     <row r="129" ht="12.75" customHeight="1">
-      <c r="A129" s="12"/>
-      <c r="B129" s="15"/>
-      <c r="C129" s="16"/>
+      <c r="A129" s="13"/>
+      <c r="B129" s="14"/>
+      <c r="C129" s="15"/>
       <c r="D129" s="5"/>
     </row>
     <row r="130" ht="12.75" customHeight="1">
-      <c r="A130" s="12"/>
-      <c r="B130" s="15"/>
-      <c r="C130" s="16"/>
+      <c r="A130" s="13"/>
+      <c r="B130" s="14"/>
+      <c r="C130" s="15"/>
       <c r="D130" s="5"/>
     </row>
     <row r="131" ht="12.75" customHeight="1">
-      <c r="A131" s="12"/>
-      <c r="B131" s="15"/>
-      <c r="C131" s="16"/>
+      <c r="A131" s="13"/>
+      <c r="B131" s="14"/>
+      <c r="C131" s="15"/>
       <c r="D131" s="5"/>
     </row>
     <row r="132" ht="12.75" customHeight="1">
-      <c r="A132" s="12"/>
-      <c r="B132" s="15"/>
-      <c r="C132" s="16"/>
+      <c r="A132" s="13"/>
+      <c r="B132" s="14"/>
+      <c r="C132" s="15"/>
       <c r="D132" s="5"/>
     </row>
     <row r="133" ht="12.75" customHeight="1">
-      <c r="A133" s="12"/>
-      <c r="B133" s="15"/>
-      <c r="C133" s="16"/>
+      <c r="A133" s="13"/>
+      <c r="B133" s="14"/>
+      <c r="C133" s="15"/>
       <c r="D133" s="5"/>
     </row>
     <row r="134" ht="12.75" customHeight="1">
-      <c r="A134" s="12"/>
-      <c r="B134" s="15"/>
-      <c r="C134" s="16"/>
+      <c r="A134" s="13"/>
+      <c r="B134" s="14"/>
+      <c r="C134" s="15"/>
       <c r="D134" s="5"/>
     </row>
     <row r="135" ht="12.75" customHeight="1">
-      <c r="A135" s="12"/>
-      <c r="B135" s="15"/>
-      <c r="C135" s="16"/>
+      <c r="A135" s="13"/>
+      <c r="B135" s="14"/>
+      <c r="C135" s="15"/>
       <c r="D135" s="5"/>
     </row>
     <row r="136" ht="12.75" customHeight="1">
-      <c r="A136" s="12"/>
-      <c r="B136" s="15"/>
-      <c r="C136" s="16"/>
+      <c r="A136" s="13"/>
+      <c r="B136" s="14"/>
+      <c r="C136" s="15"/>
       <c r="D136" s="5"/>
     </row>
     <row r="137" ht="12.75" customHeight="1">
-      <c r="A137" s="12"/>
-      <c r="B137" s="15"/>
-      <c r="C137" s="16"/>
+      <c r="A137" s="13"/>
+      <c r="B137" s="14"/>
+      <c r="C137" s="15"/>
       <c r="D137" s="5"/>
     </row>
     <row r="138" ht="12.75" customHeight="1">
-      <c r="A138" s="12"/>
-      <c r="B138" s="15"/>
-      <c r="C138" s="16"/>
+      <c r="A138" s="13"/>
+      <c r="B138" s="14"/>
+      <c r="C138" s="15"/>
       <c r="D138" s="5"/>
     </row>
     <row r="139" ht="12.75" customHeight="1">
-      <c r="A139" s="12"/>
-      <c r="B139" s="15"/>
-      <c r="C139" s="16"/>
+      <c r="A139" s="13"/>
+      <c r="B139" s="14"/>
+      <c r="C139" s="15"/>
       <c r="D139" s="5"/>
     </row>
     <row r="140" ht="12.75" customHeight="1">
-      <c r="A140" s="12"/>
-      <c r="B140" s="15"/>
-      <c r="C140" s="16"/>
+      <c r="A140" s="13"/>
+      <c r="B140" s="14"/>
+      <c r="C140" s="15"/>
       <c r="D140" s="5"/>
     </row>
     <row r="141" ht="12.75" customHeight="1">
-      <c r="A141" s="12"/>
-      <c r="B141" s="15"/>
-      <c r="C141" s="16"/>
+      <c r="A141" s="13"/>
+      <c r="B141" s="14"/>
+      <c r="C141" s="15"/>
       <c r="D141" s="5"/>
     </row>
     <row r="142" ht="12.75" customHeight="1">
-      <c r="A142" s="12"/>
-      <c r="B142" s="15"/>
-      <c r="C142" s="16"/>
+      <c r="A142" s="13"/>
+      <c r="B142" s="14"/>
+      <c r="C142" s="15"/>
       <c r="D142" s="5"/>
     </row>
     <row r="143" ht="12.75" customHeight="1">
-      <c r="A143" s="12"/>
-      <c r="B143" s="15"/>
-      <c r="C143" s="16"/>
+      <c r="A143" s="13"/>
+      <c r="B143" s="14"/>
+      <c r="C143" s="15"/>
       <c r="D143" s="5"/>
     </row>
     <row r="144" ht="12.75" customHeight="1">
-      <c r="A144" s="12"/>
-      <c r="B144" s="15"/>
-      <c r="C144" s="16"/>
+      <c r="A144" s="13"/>
+      <c r="B144" s="14"/>
+      <c r="C144" s="15"/>
       <c r="D144" s="5"/>
     </row>
     <row r="145" ht="12.75" customHeight="1">
-      <c r="A145" s="12"/>
-      <c r="B145" s="15"/>
-      <c r="C145" s="16"/>
+      <c r="A145" s="13"/>
+      <c r="B145" s="14"/>
+      <c r="C145" s="15"/>
       <c r="D145" s="5"/>
     </row>
     <row r="146" ht="12.75" customHeight="1">
-      <c r="A146" s="12"/>
-      <c r="B146" s="15"/>
-      <c r="C146" s="16"/>
+      <c r="A146" s="13"/>
+      <c r="B146" s="14"/>
+      <c r="C146" s="15"/>
       <c r="D146" s="5"/>
     </row>
     <row r="147" ht="12.75" customHeight="1">
-      <c r="A147" s="12"/>
-      <c r="B147" s="15"/>
-      <c r="C147" s="16"/>
+      <c r="A147" s="13"/>
+      <c r="B147" s="14"/>
+      <c r="C147" s="15"/>
       <c r="D147" s="5"/>
     </row>
     <row r="148" ht="12.75" customHeight="1">
-      <c r="A148" s="12"/>
-      <c r="B148" s="15"/>
-      <c r="C148" s="16"/>
+      <c r="A148" s="13"/>
+      <c r="B148" s="14"/>
+      <c r="C148" s="15"/>
       <c r="D148" s="5"/>
     </row>
     <row r="149" ht="12.75" customHeight="1">
-      <c r="A149" s="12"/>
-      <c r="B149" s="15"/>
-      <c r="C149" s="16"/>
+      <c r="A149" s="13"/>
+      <c r="B149" s="14"/>
+      <c r="C149" s="15"/>
       <c r="D149" s="5"/>
     </row>
     <row r="150" ht="12.75" customHeight="1">
-      <c r="A150" s="12"/>
-      <c r="B150" s="15"/>
-      <c r="C150" s="16"/>
+      <c r="A150" s="13"/>
+      <c r="B150" s="14"/>
+      <c r="C150" s="15"/>
       <c r="D150" s="5"/>
     </row>
     <row r="151" ht="12.75" customHeight="1">
-      <c r="A151" s="12"/>
-      <c r="B151" s="15"/>
-      <c r="C151" s="16"/>
+      <c r="A151" s="13"/>
+      <c r="B151" s="14"/>
+      <c r="C151" s="15"/>
       <c r="D151" s="5"/>
     </row>
     <row r="152" ht="12.75" customHeight="1">
-      <c r="A152" s="12"/>
-      <c r="B152" s="15"/>
-      <c r="C152" s="16"/>
+      <c r="A152" s="13"/>
+      <c r="B152" s="14"/>
+      <c r="C152" s="15"/>
       <c r="D152" s="5"/>
     </row>
     <row r="153" ht="12.75" customHeight="1">
-      <c r="A153" s="12"/>
-      <c r="B153" s="15"/>
-      <c r="C153" s="16"/>
+      <c r="A153" s="13"/>
+      <c r="B153" s="14"/>
+      <c r="C153" s="15"/>
       <c r="D153" s="5"/>
     </row>
     <row r="154" ht="12.75" customHeight="1">
-      <c r="A154" s="12"/>
-      <c r="B154" s="15"/>
-      <c r="C154" s="16"/>
+      <c r="A154" s="13"/>
+      <c r="B154" s="14"/>
+      <c r="C154" s="15"/>
       <c r="D154" s="5"/>
     </row>
     <row r="155" ht="12.75" customHeight="1">
-      <c r="A155" s="12"/>
-      <c r="B155" s="15"/>
-      <c r="C155" s="16"/>
+      <c r="A155" s="13"/>
+      <c r="B155" s="14"/>
+      <c r="C155" s="15"/>
       <c r="D155" s="5"/>
     </row>
     <row r="156" ht="12.75" customHeight="1">
-      <c r="A156" s="12"/>
-      <c r="B156" s="15"/>
-      <c r="C156" s="16"/>
+      <c r="A156" s="13"/>
+      <c r="B156" s="14"/>
+      <c r="C156" s="15"/>
       <c r="D156" s="5"/>
     </row>
     <row r="157" ht="12.75" customHeight="1">
-      <c r="A157" s="12"/>
-      <c r="B157" s="15"/>
-      <c r="C157" s="16"/>
+      <c r="A157" s="13"/>
+      <c r="B157" s="14"/>
+      <c r="C157" s="15"/>
       <c r="D157" s="5"/>
     </row>
     <row r="158" ht="12.75" customHeight="1">
-      <c r="A158" s="12"/>
-      <c r="B158" s="15"/>
-      <c r="C158" s="16"/>
+      <c r="A158" s="13"/>
+      <c r="B158" s="14"/>
+      <c r="C158" s="15"/>
       <c r="D158" s="5"/>
     </row>
     <row r="159" ht="12.75" customHeight="1">
-      <c r="A159" s="12"/>
-      <c r="B159" s="15"/>
-      <c r="C159" s="16"/>
+      <c r="A159" s="13"/>
+      <c r="B159" s="14"/>
+      <c r="C159" s="15"/>
       <c r="D159" s="5"/>
     </row>
     <row r="160" ht="12.75" customHeight="1">
-      <c r="A160" s="12"/>
-      <c r="B160" s="15"/>
-      <c r="C160" s="16"/>
+      <c r="A160" s="13"/>
+      <c r="B160" s="14"/>
+      <c r="C160" s="15"/>
       <c r="D160" s="5"/>
     </row>
     <row r="161" ht="12.75" customHeight="1">
-      <c r="A161" s="12"/>
-      <c r="B161" s="15"/>
-      <c r="C161" s="16"/>
+      <c r="A161" s="13"/>
+      <c r="B161" s="14"/>
+      <c r="C161" s="15"/>
       <c r="D161" s="5"/>
     </row>
     <row r="162" ht="12.75" customHeight="1">
-      <c r="A162" s="12"/>
-      <c r="B162" s="15"/>
-      <c r="C162" s="16"/>
+      <c r="A162" s="13"/>
+      <c r="B162" s="14"/>
+      <c r="C162" s="15"/>
       <c r="D162" s="5"/>
     </row>
     <row r="163" ht="12.75" customHeight="1">
-      <c r="A163" s="12"/>
-      <c r="B163" s="15"/>
-      <c r="C163" s="16"/>
+      <c r="A163" s="13"/>
+      <c r="B163" s="14"/>
+      <c r="C163" s="15"/>
       <c r="D163" s="5"/>
     </row>
     <row r="164" ht="12.75" customHeight="1">
-      <c r="A164" s="12"/>
-      <c r="B164" s="15"/>
-      <c r="C164" s="16"/>
+      <c r="A164" s="13"/>
+      <c r="B164" s="14"/>
+      <c r="C164" s="15"/>
       <c r="D164" s="5"/>
     </row>
     <row r="165" ht="12.75" customHeight="1">
-      <c r="A165" s="12"/>
-      <c r="B165" s="15"/>
-      <c r="C165" s="16"/>
+      <c r="A165" s="13"/>
+      <c r="B165" s="14"/>
+      <c r="C165" s="15"/>
       <c r="D165" s="5"/>
     </row>
     <row r="166" ht="12.75" customHeight="1">
-      <c r="A166" s="12"/>
-      <c r="B166" s="15"/>
-      <c r="C166" s="16"/>
+      <c r="A166" s="13"/>
+      <c r="B166" s="14"/>
+      <c r="C166" s="15"/>
       <c r="D166" s="5"/>
     </row>
     <row r="167" ht="12.75" customHeight="1">
-      <c r="A167" s="12"/>
-      <c r="B167" s="15"/>
-      <c r="C167" s="16"/>
+      <c r="A167" s="13"/>
+      <c r="B167" s="14"/>
+      <c r="C167" s="15"/>
       <c r="D167" s="5"/>
     </row>
     <row r="168" ht="12.75" customHeight="1">
-      <c r="A168" s="12"/>
-      <c r="B168" s="15"/>
-      <c r="C168" s="16"/>
+      <c r="A168" s="13"/>
+      <c r="B168" s="14"/>
+      <c r="C168" s="15"/>
       <c r="D168" s="5"/>
     </row>
     <row r="169" ht="12.75" customHeight="1">
-      <c r="A169" s="12"/>
-      <c r="B169" s="15"/>
-      <c r="C169" s="16"/>
+      <c r="A169" s="13"/>
+      <c r="B169" s="14"/>
+      <c r="C169" s="15"/>
       <c r="D169" s="5"/>
     </row>
     <row r="170" ht="12.75" customHeight="1">
-      <c r="A170" s="12"/>
-      <c r="B170" s="15"/>
-      <c r="C170" s="16"/>
+      <c r="A170" s="13"/>
+      <c r="B170" s="14"/>
+      <c r="C170" s="15"/>
       <c r="D170" s="5"/>
     </row>
     <row r="171" ht="12.75" customHeight="1">
-      <c r="A171" s="12"/>
-      <c r="B171" s="15"/>
-      <c r="C171" s="16"/>
+      <c r="A171" s="13"/>
+      <c r="B171" s="14"/>
+      <c r="C171" s="15"/>
       <c r="D171" s="5"/>
     </row>
     <row r="172" ht="12.75" customHeight="1">
-      <c r="A172" s="12"/>
-      <c r="B172" s="15"/>
-      <c r="C172" s="16"/>
+      <c r="A172" s="13"/>
+      <c r="B172" s="14"/>
+      <c r="C172" s="15"/>
       <c r="D172" s="5"/>
     </row>
     <row r="173" ht="12.75" customHeight="1">
-      <c r="A173" s="12"/>
-      <c r="B173" s="15"/>
-      <c r="C173" s="16"/>
+      <c r="A173" s="13"/>
+      <c r="B173" s="14"/>
+      <c r="C173" s="15"/>
       <c r="D173" s="5"/>
     </row>
     <row r="174" ht="12.75" customHeight="1">
-      <c r="A174" s="12"/>
-      <c r="B174" s="15"/>
-      <c r="C174" s="16"/>
+      <c r="A174" s="13"/>
+      <c r="B174" s="14"/>
+      <c r="C174" s="15"/>
       <c r="D174" s="5"/>
     </row>
     <row r="175" ht="12.75" customHeight="1">
-      <c r="A175" s="12"/>
-      <c r="B175" s="15"/>
-      <c r="C175" s="16"/>
+      <c r="A175" s="13"/>
+      <c r="B175" s="14"/>
+      <c r="C175" s="15"/>
       <c r="D175" s="5"/>
     </row>
     <row r="176" ht="12.75" customHeight="1">
-      <c r="A176" s="12"/>
-      <c r="B176" s="15"/>
-      <c r="C176" s="16"/>
+      <c r="A176" s="13"/>
+      <c r="B176" s="14"/>
+      <c r="C176" s="15"/>
       <c r="D176" s="5"/>
     </row>
     <row r="177" ht="12.75" customHeight="1">
-      <c r="B177" s="15"/>
-      <c r="C177" s="16"/>
+      <c r="B177" s="14"/>
+      <c r="C177" s="15"/>
       <c r="D177" s="5"/>
     </row>
     <row r="178" ht="12.75" customHeight="1">
-      <c r="B178" s="15"/>
-      <c r="C178" s="16"/>
+      <c r="B178" s="14"/>
+      <c r="C178" s="15"/>
       <c r="D178" s="5"/>
     </row>
     <row r="179" ht="12.75" customHeight="1">
-      <c r="B179" s="15"/>
-      <c r="C179" s="16"/>
+      <c r="B179" s="14"/>
+      <c r="C179" s="15"/>
       <c r="D179" s="5"/>
     </row>
     <row r="180" ht="12.75" customHeight="1">
-      <c r="B180" s="15"/>
-      <c r="C180" s="16"/>
+      <c r="B180" s="14"/>
+      <c r="C180" s="15"/>
       <c r="D180" s="5"/>
     </row>
     <row r="181" ht="12.75" customHeight="1">
-      <c r="B181" s="15"/>
-      <c r="C181" s="16"/>
+      <c r="B181" s="14"/>
+      <c r="C181" s="15"/>
       <c r="D181" s="5"/>
     </row>
     <row r="182" ht="12.75" customHeight="1">
-      <c r="B182" s="15"/>
-      <c r="C182" s="16"/>
+      <c r="B182" s="14"/>
+      <c r="C182" s="15"/>
       <c r="D182" s="5"/>
     </row>
     <row r="183" ht="12.75" customHeight="1">
-      <c r="B183" s="15"/>
-      <c r="C183" s="16"/>
+      <c r="B183" s="14"/>
+      <c r="C183" s="15"/>
       <c r="D183" s="5"/>
     </row>
     <row r="184" ht="12.75" customHeight="1">
-      <c r="B184" s="15"/>
-      <c r="C184" s="16"/>
+      <c r="B184" s="14"/>
+      <c r="C184" s="15"/>
       <c r="D184" s="5"/>
     </row>
     <row r="185" ht="12.75" customHeight="1">
-      <c r="B185" s="15"/>
-      <c r="C185" s="16"/>
+      <c r="B185" s="14"/>
+      <c r="C185" s="15"/>
       <c r="D185" s="5"/>
     </row>
     <row r="186" ht="12.75" customHeight="1">
-      <c r="B186" s="15"/>
-      <c r="C186" s="16"/>
+      <c r="B186" s="14"/>
+      <c r="C186" s="15"/>
       <c r="D186" s="5"/>
     </row>
     <row r="187" ht="12.75" customHeight="1">
-      <c r="B187" s="15"/>
-      <c r="C187" s="16"/>
+      <c r="B187" s="14"/>
+      <c r="C187" s="15"/>
       <c r="D187" s="5"/>
     </row>
     <row r="188" ht="12.75" customHeight="1">
-      <c r="B188" s="15"/>
-      <c r="C188" s="16"/>
+      <c r="B188" s="14"/>
+      <c r="C188" s="15"/>
       <c r="D188" s="5"/>
     </row>
     <row r="189" ht="12.75" customHeight="1">
-      <c r="B189" s="15"/>
-      <c r="C189" s="16"/>
+      <c r="B189" s="14"/>
+      <c r="C189" s="15"/>
       <c r="D189" s="5"/>
     </row>
     <row r="190" ht="12.75" customHeight="1">
-      <c r="B190" s="15"/>
-      <c r="C190" s="16"/>
+      <c r="B190" s="14"/>
+      <c r="C190" s="15"/>
       <c r="D190" s="5"/>
     </row>
     <row r="191" ht="12.75" customHeight="1">
-      <c r="B191" s="15"/>
-      <c r="C191" s="16"/>
+      <c r="B191" s="14"/>
+      <c r="C191" s="15"/>
       <c r="D191" s="5"/>
     </row>
     <row r="192" ht="12.75" customHeight="1">
-      <c r="B192" s="15"/>
-      <c r="C192" s="16"/>
+      <c r="B192" s="14"/>
+      <c r="C192" s="15"/>
       <c r="D192" s="5"/>
     </row>
     <row r="193" ht="12.75" customHeight="1">
-      <c r="B193" s="15"/>
-      <c r="C193" s="16"/>
+      <c r="B193" s="14"/>
+      <c r="C193" s="15"/>
       <c r="D193" s="5"/>
     </row>
     <row r="194" ht="12.75" customHeight="1">
-      <c r="B194" s="15"/>
-      <c r="C194" s="16"/>
+      <c r="B194" s="14"/>
+      <c r="C194" s="15"/>
       <c r="D194" s="5"/>
     </row>
     <row r="195" ht="12.75" customHeight="1">
-      <c r="B195" s="15"/>
-      <c r="C195" s="16"/>
+      <c r="B195" s="14"/>
+      <c r="C195" s="15"/>
       <c r="D195" s="5"/>
     </row>
     <row r="196" ht="12.75" customHeight="1">
-      <c r="B196" s="15"/>
-      <c r="C196" s="16"/>
+      <c r="B196" s="14"/>
+      <c r="C196" s="15"/>
       <c r="D196" s="5"/>
     </row>
     <row r="197" ht="12.75" customHeight="1">
-      <c r="B197" s="15"/>
-      <c r="C197" s="16"/>
+      <c r="B197" s="14"/>
+      <c r="C197" s="15"/>
       <c r="D197" s="5"/>
     </row>
     <row r="198" ht="12.75" customHeight="1">
-      <c r="B198" s="15"/>
-      <c r="C198" s="16"/>
+      <c r="B198" s="14"/>
+      <c r="C198" s="15"/>
       <c r="D198" s="5"/>
     </row>
     <row r="199" ht="12.75" customHeight="1">
-      <c r="B199" s="15"/>
-      <c r="C199" s="16"/>
+      <c r="B199" s="14"/>
+      <c r="C199" s="15"/>
       <c r="D199" s="5"/>
     </row>
     <row r="200" ht="12.75" customHeight="1">
-      <c r="B200" s="15"/>
-      <c r="C200" s="16"/>
+      <c r="B200" s="14"/>
+      <c r="C200" s="15"/>
       <c r="D200" s="5"/>
     </row>
     <row r="201" ht="12.75" customHeight="1">
-      <c r="B201" s="15"/>
-      <c r="C201" s="16"/>
+      <c r="B201" s="14"/>
+      <c r="C201" s="15"/>
       <c r="D201" s="5"/>
     </row>
     <row r="202" ht="12.75" customHeight="1">
-      <c r="B202" s="15"/>
-      <c r="C202" s="16"/>
+      <c r="B202" s="14"/>
+      <c r="C202" s="15"/>
       <c r="D202" s="5"/>
     </row>
     <row r="203" ht="12.75" customHeight="1">
-      <c r="B203" s="15"/>
-      <c r="C203" s="16"/>
+      <c r="B203" s="14"/>
+      <c r="C203" s="15"/>
       <c r="D203" s="5"/>
     </row>
     <row r="204" ht="12.75" customHeight="1">
-      <c r="B204" s="15"/>
-      <c r="C204" s="16"/>
+      <c r="B204" s="14"/>
+      <c r="C204" s="15"/>
       <c r="D204" s="5"/>
     </row>
     <row r="205" ht="12.75" customHeight="1">
-      <c r="B205" s="15"/>
-      <c r="C205" s="16"/>
+      <c r="B205" s="14"/>
+      <c r="C205" s="15"/>
       <c r="D205" s="5"/>
     </row>
     <row r="206" ht="12.75" customHeight="1">
-      <c r="B206" s="15"/>
-      <c r="C206" s="16"/>
+      <c r="B206" s="14"/>
+      <c r="C206" s="15"/>
       <c r="D206" s="5"/>
     </row>
     <row r="207" ht="12.75" customHeight="1">
-      <c r="B207" s="15"/>
-      <c r="C207" s="16"/>
+      <c r="B207" s="14"/>
+      <c r="C207" s="15"/>
       <c r="D207" s="5"/>
     </row>
     <row r="208" ht="12.75" customHeight="1">
-      <c r="B208" s="15"/>
-      <c r="C208" s="16"/>
+      <c r="B208" s="14"/>
+      <c r="C208" s="15"/>
       <c r="D208" s="5"/>
     </row>
     <row r="209" ht="12.75" customHeight="1">
-      <c r="B209" s="15"/>
-      <c r="C209" s="16"/>
+      <c r="B209" s="14"/>
+      <c r="C209" s="15"/>
       <c r="D209" s="5"/>
     </row>
     <row r="210" ht="12.75" customHeight="1">
-      <c r="B210" s="15"/>
-      <c r="C210" s="16"/>
+      <c r="B210" s="14"/>
+      <c r="C210" s="15"/>
       <c r="D210" s="5"/>
     </row>
     <row r="211" ht="12.75" customHeight="1">
-      <c r="B211" s="15"/>
-      <c r="C211" s="16"/>
+      <c r="B211" s="14"/>
+      <c r="C211" s="15"/>
       <c r="D211" s="5"/>
     </row>
     <row r="212" ht="12.75" customHeight="1">
-      <c r="B212" s="15"/>
-      <c r="C212" s="16"/>
+      <c r="B212" s="14"/>
+      <c r="C212" s="15"/>
       <c r="D212" s="5"/>
     </row>
     <row r="213" ht="12.75" customHeight="1">
-      <c r="B213" s="15"/>
-      <c r="C213" s="16"/>
+      <c r="B213" s="14"/>
+      <c r="C213" s="15"/>
       <c r="D213" s="5"/>
     </row>
     <row r="214" ht="12.75" customHeight="1">
-      <c r="B214" s="15"/>
-      <c r="C214" s="16"/>
+      <c r="B214" s="14"/>
+      <c r="C214" s="15"/>
       <c r="D214" s="5"/>
     </row>
     <row r="215" ht="12.75" customHeight="1">
-      <c r="B215" s="15"/>
-      <c r="C215" s="16"/>
+      <c r="B215" s="14"/>
+      <c r="C215" s="15"/>
       <c r="D215" s="5"/>
     </row>
     <row r="216" ht="12.75" customHeight="1">
-      <c r="B216" s="15"/>
-      <c r="C216" s="16"/>
+      <c r="B216" s="14"/>
+      <c r="C216" s="15"/>
       <c r="D216" s="5"/>
     </row>
     <row r="217" ht="12.75" customHeight="1">
-      <c r="B217" s="15"/>
-      <c r="C217" s="16"/>
+      <c r="B217" s="14"/>
+      <c r="C217" s="15"/>
       <c r="D217" s="5"/>
     </row>
     <row r="218" ht="12.75" customHeight="1">
-      <c r="B218" s="15"/>
-      <c r="C218" s="16"/>
+      <c r="B218" s="14"/>
+      <c r="C218" s="15"/>
       <c r="D218" s="5"/>
     </row>
     <row r="219" ht="12.75" customHeight="1">
-      <c r="B219" s="15"/>
-      <c r="C219" s="16"/>
+      <c r="B219" s="14"/>
+      <c r="C219" s="15"/>
       <c r="D219" s="5"/>
     </row>
     <row r="220" ht="12.75" customHeight="1">
-      <c r="B220" s="15"/>
-      <c r="C220" s="16"/>
+      <c r="B220" s="14"/>
+      <c r="C220" s="15"/>
       <c r="D220" s="5"/>
     </row>
     <row r="221" ht="12.75" customHeight="1">
-      <c r="B221" s="15"/>
-      <c r="C221" s="16"/>
+      <c r="B221" s="14"/>
+      <c r="C221" s="15"/>
       <c r="D221" s="5"/>
     </row>
     <row r="222" ht="12.75" customHeight="1">
-      <c r="B222" s="15"/>
-      <c r="C222" s="16"/>
+      <c r="B222" s="14"/>
+      <c r="C222" s="15"/>
       <c r="D222" s="5"/>
     </row>
     <row r="223" ht="12.75" customHeight="1">
-      <c r="B223" s="15"/>
-      <c r="C223" s="16"/>
+      <c r="B223" s="14"/>
+      <c r="C223" s="15"/>
       <c r="D223" s="5"/>
     </row>
     <row r="224" ht="12.75" customHeight="1">
-      <c r="B224" s="15"/>
-      <c r="C224" s="16"/>
+      <c r="B224" s="14"/>
+      <c r="C224" s="15"/>
       <c r="D224" s="5"/>
     </row>
     <row r="225" ht="12.75" customHeight="1">
-      <c r="B225" s="15"/>
-      <c r="C225" s="16"/>
+      <c r="B225" s="14"/>
+      <c r="C225" s="15"/>
       <c r="D225" s="5"/>
     </row>
     <row r="226" ht="12.75" customHeight="1">
-      <c r="B226" s="15"/>
-      <c r="C226" s="16"/>
+      <c r="B226" s="14"/>
+      <c r="C226" s="15"/>
       <c r="D226" s="5"/>
     </row>
     <row r="227" ht="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
add comments and log messages
</commit_message>
<xml_diff>
--- a/files/grid.xlsx
+++ b/files/grid.xlsx
@@ -1199,9 +1199,7 @@
       <c r="C66" s="4">
         <v>3.0</v>
       </c>
-      <c r="D66" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="D66" s="12"/>
     </row>
     <row r="67" ht="12.75" customHeight="1">
       <c r="A67" s="10">
@@ -1213,9 +1211,7 @@
       <c r="C67" s="4">
         <v>3.0</v>
       </c>
-      <c r="D67" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D67" s="12"/>
     </row>
     <row r="68" ht="12.75" customHeight="1">
       <c r="A68" s="10">
@@ -1227,9 +1223,7 @@
       <c r="C68" s="4">
         <v>3.0</v>
       </c>
-      <c r="D68" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D68" s="12"/>
     </row>
     <row r="69" ht="12.75" customHeight="1">
       <c r="A69" s="10">
@@ -1241,9 +1235,7 @@
       <c r="C69" s="4">
         <v>3.0</v>
       </c>
-      <c r="D69" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D69" s="12"/>
     </row>
     <row r="70" ht="12.75" customHeight="1">
       <c r="A70" s="10">
@@ -1255,9 +1247,7 @@
       <c r="C70" s="4">
         <v>3.0</v>
       </c>
-      <c r="D70" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D70" s="12"/>
     </row>
     <row r="71" ht="12.75" customHeight="1">
       <c r="A71" s="10">
@@ -1269,9 +1259,7 @@
       <c r="C71" s="4">
         <v>3.0</v>
       </c>
-      <c r="D71" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D71" s="12"/>
     </row>
     <row r="72" ht="12.75" customHeight="1">
       <c r="A72" s="10">
@@ -1283,9 +1271,7 @@
       <c r="C72" s="4">
         <v>3.0</v>
       </c>
-      <c r="D72" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D72" s="12"/>
     </row>
     <row r="73" ht="12.75" customHeight="1">
       <c r="A73" s="10">
@@ -1297,9 +1283,7 @@
       <c r="C73" s="4">
         <v>3.0</v>
       </c>
-      <c r="D73" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D73" s="12"/>
     </row>
     <row r="74" ht="12.75" customHeight="1">
       <c r="A74" s="10">
@@ -1311,9 +1295,7 @@
       <c r="C74" s="4">
         <v>3.0</v>
       </c>
-      <c r="D74" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D74" s="12"/>
     </row>
     <row r="75" ht="12.75" customHeight="1">
       <c r="A75" s="10">
@@ -1325,9 +1307,7 @@
       <c r="C75" s="4">
         <v>3.0</v>
       </c>
-      <c r="D75" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D75" s="12"/>
     </row>
     <row r="76" ht="12.75" customHeight="1">
       <c r="A76" s="10">
@@ -1339,9 +1319,7 @@
       <c r="C76" s="4">
         <v>3.0</v>
       </c>
-      <c r="D76" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="D76" s="12"/>
     </row>
     <row r="77" ht="12.75" customHeight="1">
       <c r="A77" s="10">
@@ -1353,7 +1331,7 @@
       <c r="C77" s="4">
         <v>3.0</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1367,7 +1345,9 @@
       <c r="C78" s="4">
         <v>3.0</v>
       </c>
-      <c r="D78" s="5"/>
+      <c r="D78" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="79" ht="12.75" customHeight="1">
       <c r="A79" s="10">
@@ -1379,7 +1359,9 @@
       <c r="C79" s="4">
         <v>3.0</v>
       </c>
-      <c r="D79" s="5"/>
+      <c r="D79" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="80" ht="12.75" customHeight="1">
       <c r="A80" s="10">
@@ -1391,7 +1373,9 @@
       <c r="C80" s="4">
         <v>3.0</v>
       </c>
-      <c r="D80" s="5"/>
+      <c r="D80" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="81" ht="12.75" customHeight="1">
       <c r="A81" s="10">
@@ -1403,7 +1387,9 @@
       <c r="C81" s="4">
         <v>3.0</v>
       </c>
-      <c r="D81" s="5"/>
+      <c r="D81" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="82" ht="12.75" customHeight="1">
       <c r="A82" s="10">
@@ -1415,7 +1401,9 @@
       <c r="C82" s="4">
         <v>3.0</v>
       </c>
-      <c r="D82" s="5"/>
+      <c r="D82" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="83" ht="12.75" customHeight="1">
       <c r="A83" s="10">
@@ -1427,7 +1415,9 @@
       <c r="C83" s="4">
         <v>3.0</v>
       </c>
-      <c r="D83" s="5"/>
+      <c r="D83" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="84" ht="12.75" customHeight="1">
       <c r="A84" s="10">
@@ -1439,7 +1429,9 @@
       <c r="C84" s="4">
         <v>3.0</v>
       </c>
-      <c r="D84" s="5"/>
+      <c r="D84" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="85" ht="12.75" customHeight="1">
       <c r="A85" s="10">
@@ -1451,7 +1443,9 @@
       <c r="C85" s="4">
         <v>3.0</v>
       </c>
-      <c r="D85" s="5"/>
+      <c r="D85" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="86" ht="12.75" customHeight="1">
       <c r="A86" s="10">
@@ -1463,7 +1457,9 @@
       <c r="C86" s="4">
         <v>3.0</v>
       </c>
-      <c r="D86" s="5"/>
+      <c r="D86" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="87" ht="12.75" customHeight="1">
       <c r="A87" s="10">
@@ -1475,7 +1471,9 @@
       <c r="C87" s="4">
         <v>3.0</v>
       </c>
-      <c r="D87" s="5"/>
+      <c r="D87" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="88" ht="12.75" customHeight="1">
       <c r="A88" s="10">
@@ -1487,7 +1485,9 @@
       <c r="C88" s="4">
         <v>3.0</v>
       </c>
-      <c r="D88" s="5"/>
+      <c r="D88" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="89" ht="12.75" customHeight="1">
       <c r="A89" s="10">

</xml_diff>